<commit_message>
loading prescription data from file, use XSSF excel workbooks, added prescriptions.xlsx. fixed issue with primary keys, no longer try to set ID in data.sql
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/medications.xlsx
+++ b/src/main/resources/initialDataFiles/medications.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\InitialDataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F65FCC5F-7C30-4309-A83A-E68DD1CA26F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B0DBE4-849C-4CDA-AA69-1E2482BE82F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3010" yWindow="-110" windowWidth="35500" windowHeight="21820" xr2:uid="{67251941-77B2-4AC4-9CF8-C86461879E3F}"/>
+    <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{67251941-77B2-4AC4-9CF8-C86461879E3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Foo</t>
+    <t>FOO</t>
   </si>
   <si>
-    <t>Bar</t>
+    <t>BAR</t>
+  </si>
+  <si>
+    <t>FOOBAR</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D499C32-2FAA-4AC9-A61F-5C1B4153A4C7}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -411,6 +414,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>